<commit_message>
commit Jostens local test suite
</commit_message>
<xml_diff>
--- a/src/main/java/com/jostens/qa/testdata/Jostens.xlsx
+++ b/src/main/java/com/jostens/qa/testdata/Jostens.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="213">
   <si>
     <t>Website</t>
   </si>
@@ -584,6 +584,87 @@
   </si>
   <si>
     <t>Success - 2020/12/19 02:34:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 11:58:30</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 11:58:33</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 11:58:36</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 11:58:39</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/19 11:59:05</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/19 11:59:17</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/19 11:59:30</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/19 11:59:32</t>
+  </si>
+  <si>
+    <t>Failure - 2020/12/19 11:59:33</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 11:59:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 11:59:54</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:00:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:00:02</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:00:12</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:01:53</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:01:56</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:01:59</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:02:01</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:02:27</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:02:48</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:03:09</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:03:11</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:03:21</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:03:32</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:03:39</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:03:40</t>
+  </si>
+  <si>
+    <t>Success - 2020/12/19 12:03:50</t>
   </si>
 </sst>
 </file>
@@ -976,7 +1057,7 @@
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,7 +1080,7 @@
         <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1045,7 +1126,7 @@
         <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,7 +1137,7 @@
         <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1150,7 +1231,7 @@
         <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1185,7 +1266,7 @@
         <v>82</v>
       </c>
       <c r="K3" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1220,7 +1301,7 @@
         <v>82</v>
       </c>
       <c r="K4" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1288,7 +1369,7 @@
         <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1311,7 +1392,7 @@
         <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1334,7 +1415,7 @@
         <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1546,7 @@
         <v>53</v>
       </c>
       <c r="P2" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1515,7 +1596,7 @@
         <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1565,7 +1646,7 @@
         <v>53</v>
       </c>
       <c r="P4" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1622,7 +1703,7 @@
         <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>115</v>

</xml_diff>